<commit_message>
Update the workflow to include multiple languages
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kechun/GitHub/InTone_Visualisation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51899FE0-44F7-564F-8CE2-2F94EC6B9BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3A5790-78C4-D941-9233-E6E3494FA5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="-18880" windowWidth="26840" windowHeight="14600" xr2:uid="{2CAB8BCF-BC3F-8841-8F87-92B696A48E11}"/>
+    <workbookView xWindow="1620" yWindow="-19140" windowWidth="26840" windowHeight="14600" activeTab="2" xr2:uid="{2CAB8BCF-BC3F-8841-8F87-92B696A48E11}"/>
   </bookViews>
   <sheets>
     <sheet name="Cantonese" sheetId="1" r:id="rId1"/>
+    <sheet name="Chengdu" sheetId="2" r:id="rId2"/>
+    <sheet name="Changsha" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="206">
   <si>
     <t>Label</t>
   </si>
@@ -472,12 +474,326 @@
   <si>
     <t>Sen_index</t>
   </si>
+  <si>
+    <t>小英捏了个狮子</t>
+  </si>
+  <si>
+    <t>A2a</t>
+  </si>
+  <si>
+    <t>是小英捏了个狮子，不是小刚</t>
+  </si>
+  <si>
+    <t>小英手工好差嘛。连小英都捏了个狮子，你咋个啥子都做不出来喃</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>小银拿了个篮子</t>
+  </si>
+  <si>
+    <t>B2a</t>
+  </si>
+  <si>
+    <t>是小银拿了个篮子，不是小明</t>
+  </si>
+  <si>
+    <t>小银对集体活动从来都不热心。连小银都拿了个篮子，这次活动肯定很隆重</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <r>
+      <t>小影买了</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>把</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>椅子</t>
+    </r>
+  </si>
+  <si>
+    <t>C2a</t>
+  </si>
+  <si>
+    <r>
+      <t>是小影买了</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>把</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>椅子，不是小雨</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>小影平时抠得很。连小影都买了</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>把</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>椅子，这家铺子肯定很相因</t>
+    </r>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>小映买了双袜子</t>
+  </si>
+  <si>
+    <t>D2a</t>
+  </si>
+  <si>
+    <t>是小映卖了双袜子，不是小丽</t>
+  </si>
+  <si>
+    <t>小映嘴巴笨得很。连小映都卖了双袜子，你咋个啥子都没卖出去</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>小映卖了双袜子</t>
+  </si>
+  <si>
+    <t>连小英都捏了个狮子</t>
+  </si>
+  <si>
+    <t>连小银都拿了个篮子</t>
+  </si>
+  <si>
+    <r>
+      <t>连小影都买了</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>把</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>椅子</t>
+    </r>
+  </si>
+  <si>
+    <t>连小映都卖了双袜子</t>
+  </si>
+  <si>
+    <t>Name(prefix),Name,Verb,Aspect,Classifier,Object, Object(suffix)</t>
+  </si>
+  <si>
+    <t>COP,Name(prefix),Name,Verb,Aspect,Classifier,Object, Object(suffix),Neg,COP,Person,Person</t>
+  </si>
+  <si>
+    <t>LIN,Name(prefix),Name,DOU,Verb,Aspect,Classifier,Object, Object(suffix)</t>
+  </si>
+  <si>
+    <t>0,1,2,3,4,5,6,7,8,9,10,11</t>
+  </si>
+  <si>
+    <t>小英开哒杂椰子</t>
+  </si>
+  <si>
+    <t>是小英开哒杂椰子，不是小刚</t>
+  </si>
+  <si>
+    <t>小英瓜瘦滴。连小英都开哒杂椰子，你也要克搞两下啵</t>
+  </si>
+  <si>
+    <t>小莹提哒杂篮子</t>
+  </si>
+  <si>
+    <t>是小莹提哒杂篮子，不是小明</t>
+  </si>
+  <si>
+    <t>小莹对集体活动从来都不热心。连小莹都提哒杂篮子，果次活动肯定很热闹咯</t>
+  </si>
+  <si>
+    <t>小影买哒杂李子</t>
+  </si>
+  <si>
+    <t>是小影买哒杂李子，不是小雨</t>
+  </si>
+  <si>
+    <t>小影有蛮抠啦。连小影都买哒杂李子，她肯定在这家铺子捡哒一杂好大的篓子。</t>
+  </si>
+  <si>
+    <t>小映卖哒杂柚子</t>
+  </si>
+  <si>
+    <t>是小映卖哒杂柚子，不是小丽</t>
+  </si>
+  <si>
+    <t>小映连不灵泛。连小映都卖哒杂柚子，你哦该木子都没卖出去。</t>
+  </si>
+  <si>
+    <t>小映卖哒杂柚子。</t>
+  </si>
+  <si>
+    <t>小梦烂哒杂柜子</t>
+  </si>
+  <si>
+    <t>E2a</t>
+  </si>
+  <si>
+    <t>小梦最爱惜家伙哒。连小梦都烂哒杂柜子，你也要注意点啊子啵。</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>小岳喫哒杂鸭子</t>
+  </si>
+  <si>
+    <t>F2a</t>
+  </si>
+  <si>
+    <t>是小岳喫哒杂鸭子，不是小陆</t>
+  </si>
+  <si>
+    <t>小岳口胃不大。连小岳都喫哒杂鸭子，你哦该木子都么喫</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>连小英都开哒杂椰子</t>
+  </si>
+  <si>
+    <t>连小莹都提哒杂篮子</t>
+  </si>
+  <si>
+    <t>连小影都买哒杂李子</t>
+  </si>
+  <si>
+    <t>连小映都卖哒杂柚子</t>
+  </si>
+  <si>
+    <t>是小英捏了个狮子不是小刚</t>
+  </si>
+  <si>
+    <t>是小银拿了个篮子不是小明</t>
+  </si>
+  <si>
+    <r>
+      <t>是小影买了</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>把</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>椅子不是小雨</t>
+    </r>
+  </si>
+  <si>
+    <t>是小映卖了双袜子不是小丽</t>
+  </si>
+  <si>
+    <t>连小梦都烂哒杂柜子</t>
+  </si>
+  <si>
+    <t>是小岳喫哒杂鸭子不是小陆</t>
+  </si>
+  <si>
+    <t>连小岳都喫哒杂鸭子</t>
+  </si>
+  <si>
+    <t>是小英开哒杂椰子不是小刚</t>
+  </si>
+  <si>
+    <t>是小莹提哒杂篮子不是小明</t>
+  </si>
+  <si>
+    <t>是小影买哒杂李子不是小雨</t>
+  </si>
+  <si>
+    <t>是小映卖哒杂柚子不是小丽</t>
+  </si>
+  <si>
+    <t>是小梦烂哒杂柜子不是小雨</t>
+  </si>
+  <si>
+    <t>是小梦烂哒杂柜子，不是小雨</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -504,6 +820,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -532,7 +862,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -541,6 +871,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -857,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5AFC9B-E0A4-1942-B387-A33AB681AEAA}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1637,4 +1972,1100 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D541A2DA-F734-AF4D-8E64-EA40FED098DC}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="35.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" customWidth="1"/>
+    <col min="4" max="4" width="65.83203125" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" t="s">
+        <v>163</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" t="s">
+        <v>163</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" t="s">
+        <v>163</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" t="s">
+        <v>163</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D22" t="s">
+        <v>163</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D23" t="s">
+        <v>164</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D24" t="s">
+        <v>165</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" t="s">
+        <v>163</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C20BF2F-1693-4C4C-B542-5E44C357A8C2}">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="57.1640625" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="56.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D13" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D14" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D16" t="s">
+        <v>163</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D19" t="s">
+        <v>163</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D20" t="s">
+        <v>163</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D21" t="s">
+        <v>163</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D22" t="s">
+        <v>163</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D23" t="s">
+        <v>164</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D24" t="s">
+        <v>165</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D25" t="s">
+        <v>163</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D26" t="s">
+        <v>163</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" t="s">
+        <v>163</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>181</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D28" t="s">
+        <v>163</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D29" t="s">
+        <v>164</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D30" t="s">
+        <v>165</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>183</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D31" t="s">
+        <v>163</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>185</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>188</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>